<commit_message>
Fix: Update dashboard and KPIs
</commit_message>
<xml_diff>
--- a/public/data/Pmix.xlsx
+++ b/public/data/Pmix.xlsx
@@ -2440,22 +2440,22 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>79.9414846832577</v>
+        <v>677.9061000678731</v>
       </c>
       <c r="G49" t="n">
-        <v>210.1880788764419</v>
+        <v>244.1388134236847</v>
       </c>
       <c r="H49" t="n">
         <v>141.6120002168765</v>
       </c>
       <c r="I49" t="n">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="J49" t="n">
         <v>27.5</v>
       </c>
       <c r="K49" t="n">
-        <v>-6.5</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="50">
@@ -2645,22 +2645,22 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>101.9384077601809</v>
+        <v>5773.99930088235</v>
       </c>
       <c r="G54" t="n">
-        <v>212.7183142447378</v>
+        <v>242.1331862562112</v>
       </c>
       <c r="H54" t="n">
         <v>129.2379594271063</v>
       </c>
       <c r="I54" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="J54" t="n">
         <v>24.5</v>
       </c>
       <c r="K54" t="n">
-        <v>-6.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="55">
@@ -2973,13 +2973,13 @@
         </is>
       </c>
       <c r="F62" t="n">
-        <v>493.4191988816796</v>
+        <v>495.6342526451205</v>
       </c>
       <c r="G62" t="n">
         <v>277.22153234181</v>
       </c>
       <c r="H62" t="n">
-        <v>211.5143983934183</v>
+        <v>210.8411957790392</v>
       </c>
       <c r="I62" t="n">
         <v>39.9</v>
@@ -3014,13 +3014,13 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G63" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H63" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I63" t="n">
         <v>23.05</v>
@@ -3055,13 +3055,13 @@
         </is>
       </c>
       <c r="F64" t="n">
-        <v>214.2855795785954</v>
+        <v>213.6597999528158</v>
       </c>
       <c r="G64" t="n">
         <v>0</v>
       </c>
       <c r="H64" t="n">
-        <v>214.2855795785954</v>
+        <v>213.6597999528158</v>
       </c>
       <c r="I64" t="n">
         <v>0</v>
@@ -3178,13 +3178,13 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>518.1075585011264</v>
+        <v>520.6087294613138</v>
       </c>
       <c r="G67" t="n">
         <v>277.22153234181</v>
       </c>
       <c r="H67" t="n">
-        <v>211.6231055752105</v>
+        <v>210.9419831262309</v>
       </c>
       <c r="I67" t="n">
         <v>39.9</v>
@@ -3219,13 +3219,13 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G68" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H68" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I68" t="n">
         <v>22.5</v>
@@ -3260,13 +3260,13 @@
         </is>
       </c>
       <c r="F69" t="n">
-        <v>214.573357626453</v>
+        <v>213.9446447551659</v>
       </c>
       <c r="G69" t="n">
         <v>0</v>
       </c>
       <c r="H69" t="n">
-        <v>214.573357626453</v>
+        <v>213.9446447551659</v>
       </c>
       <c r="I69" t="n">
         <v>0</v>
@@ -3383,13 +3383,13 @@
         </is>
       </c>
       <c r="F72" t="n">
-        <v>496.4346249564804</v>
+        <v>498.6846249564804</v>
       </c>
       <c r="G72" t="n">
         <v>277.22153234181</v>
       </c>
       <c r="H72" t="n">
-        <v>211.52900947357</v>
+        <v>210.8547423725928</v>
       </c>
       <c r="I72" t="n">
         <v>39.9</v>
@@ -3424,13 +3424,13 @@
         </is>
       </c>
       <c r="F73" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G73" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H73" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I73" t="n">
         <v>22.3</v>
@@ -3465,13 +3465,13 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>214.308464112413</v>
+        <v>213.6824512306345</v>
       </c>
       <c r="G74" t="n">
         <v>0</v>
       </c>
       <c r="H74" t="n">
-        <v>214.308464112413</v>
+        <v>213.6824512306345</v>
       </c>
       <c r="I74" t="n">
         <v>0</v>
@@ -3588,13 +3588,13 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>481.9792319174866</v>
+        <v>484.0617061442907</v>
       </c>
       <c r="G77" t="n">
         <v>277.22153234181</v>
       </c>
       <c r="H77" t="n">
-        <v>211.4549864516093</v>
+        <v>210.7861122794238</v>
       </c>
       <c r="I77" t="n">
         <v>39.9</v>
@@ -3629,13 +3629,13 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G78" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H78" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I78" t="n">
         <v>22</v>
@@ -3670,13 +3670,13 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>213.5934415956458</v>
+        <v>212.974716749215</v>
       </c>
       <c r="G79" t="n">
         <v>0</v>
       </c>
       <c r="H79" t="n">
-        <v>213.5934415956458</v>
+        <v>212.974716749215</v>
       </c>
       <c r="I79" t="n">
         <v>0</v>
@@ -3793,13 +3793,13 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>458.0261303564371</v>
+        <v>459.8310084052176</v>
       </c>
       <c r="G82" t="n">
         <v>277.22153234181</v>
       </c>
       <c r="H82" t="n">
-        <v>211.305765760554</v>
+        <v>210.6477630245759</v>
       </c>
       <c r="I82" t="n">
         <v>39.9</v>
@@ -3834,13 +3834,13 @@
         </is>
       </c>
       <c r="F83" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G83" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H83" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I83" t="n">
         <v>22.3</v>
@@ -3875,13 +3875,13 @@
         </is>
       </c>
       <c r="F84" t="n">
-        <v>213.0956509493548</v>
+        <v>212.4819999512866</v>
       </c>
       <c r="G84" t="n">
         <v>0</v>
       </c>
       <c r="H84" t="n">
-        <v>213.0956509493548</v>
+        <v>212.4819999512866</v>
       </c>
       <c r="I84" t="n">
         <v>0</v>
@@ -3998,13 +3998,13 @@
         </is>
       </c>
       <c r="F87" t="n">
-        <v>441.9193125743976</v>
+        <v>443.5375262346428</v>
       </c>
       <c r="G87" t="n">
         <v>277.22153234181</v>
       </c>
       <c r="H87" t="n">
-        <v>211.1804982738273</v>
+        <v>210.5316218693329</v>
       </c>
       <c r="I87" t="n">
         <v>39.9</v>
@@ -4039,13 +4039,13 @@
         </is>
       </c>
       <c r="F88" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G88" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H88" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I88" t="n">
         <v>22.1</v>
@@ -4080,13 +4080,13 @@
         </is>
       </c>
       <c r="F89" t="n">
-        <v>212.8747059095518</v>
+        <v>212.2633069458213</v>
       </c>
       <c r="G89" t="n">
         <v>0</v>
       </c>
       <c r="H89" t="n">
-        <v>212.8747059095518</v>
+        <v>212.2633069458213</v>
       </c>
       <c r="I89" t="n">
         <v>0</v>
@@ -4203,13 +4203,13 @@
         </is>
       </c>
       <c r="F92" t="n">
-        <v>442.7134050614781</v>
+        <v>444.3408215816889</v>
       </c>
       <c r="G92" t="n">
         <v>277.22153234181</v>
       </c>
       <c r="H92" t="n">
-        <v>211.1872577432889</v>
+        <v>210.5378888793338</v>
       </c>
       <c r="I92" t="n">
         <v>39.9</v>
@@ -4244,13 +4244,13 @@
         </is>
       </c>
       <c r="F93" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G93" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H93" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I93" t="n">
         <v>20.9</v>
@@ -4285,13 +4285,13 @@
         </is>
       </c>
       <c r="F94" t="n">
-        <v>212.8252567602776</v>
+        <v>212.2143618186433</v>
       </c>
       <c r="G94" t="n">
         <v>0</v>
       </c>
       <c r="H94" t="n">
-        <v>212.8252567602776</v>
+        <v>212.2143618186433</v>
       </c>
       <c r="I94" t="n">
         <v>0</v>
@@ -4408,13 +4408,13 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>450.9725455008762</v>
+        <v>452.6956784699108</v>
       </c>
       <c r="G97" t="n">
         <v>277.22153234181</v>
       </c>
       <c r="H97" t="n">
-        <v>211.253824026231</v>
+        <v>210.5996054923444</v>
       </c>
       <c r="I97" t="n">
         <v>39.9</v>
@@ -4449,13 +4449,13 @@
         </is>
       </c>
       <c r="F98" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G98" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H98" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I98" t="n">
         <v>21.6</v>
@@ -4490,13 +4490,13 @@
         </is>
       </c>
       <c r="F99" t="n">
-        <v>213.111915420091</v>
+        <v>212.4980986425754</v>
       </c>
       <c r="G99" t="n">
         <v>0</v>
       </c>
       <c r="H99" t="n">
-        <v>213.111915420091</v>
+        <v>212.4980986425754</v>
       </c>
       <c r="I99" t="n">
         <v>0</v>
@@ -4613,13 +4613,13 @@
         </is>
       </c>
       <c r="F102" t="n">
-        <v>476.6059141009717</v>
+        <v>478.6261161211738</v>
       </c>
       <c r="G102" t="n">
         <v>277.22153234181</v>
       </c>
       <c r="H102" t="n">
-        <v>211.4246863612867</v>
+        <v>210.75801969462</v>
       </c>
       <c r="I102" t="n">
         <v>39.9</v>
@@ -4654,13 +4654,13 @@
         </is>
       </c>
       <c r="F103" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G103" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H103" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I103" t="n">
         <v>22</v>
@@ -4695,13 +4695,13 @@
         </is>
       </c>
       <c r="F104" t="n">
-        <v>213.6092817643541</v>
+        <v>212.9903954632742</v>
       </c>
       <c r="G104" t="n">
         <v>0</v>
       </c>
       <c r="H104" t="n">
-        <v>213.6092817643541</v>
+        <v>212.9903954632742</v>
       </c>
       <c r="I104" t="n">
         <v>0</v>
@@ -4818,13 +4818,13 @@
         </is>
       </c>
       <c r="F107" t="n">
-        <v>498.2755524726061</v>
+        <v>500.5468872647287</v>
       </c>
       <c r="G107" t="n">
         <v>277.22153234181</v>
       </c>
       <c r="H107" t="n">
-        <v>211.5377305214109</v>
+        <v>210.8628280506697</v>
       </c>
       <c r="I107" t="n">
         <v>39.9</v>
@@ -4859,13 +4859,13 @@
         </is>
       </c>
       <c r="F108" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G108" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H108" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I108" t="n">
         <v>22</v>
@@ -4900,13 +4900,13 @@
         </is>
       </c>
       <c r="F109" t="n">
-        <v>213.8531000784695</v>
+        <v>213.2317286018183</v>
       </c>
       <c r="G109" t="n">
         <v>0</v>
       </c>
       <c r="H109" t="n">
-        <v>213.8531000784695</v>
+        <v>213.2317286018183</v>
       </c>
       <c r="I109" t="n">
         <v>0</v>
@@ -5023,13 +5023,13 @@
         </is>
       </c>
       <c r="F112" t="n">
-        <v>495.8263068980065</v>
+        <v>498.0692570064664</v>
       </c>
       <c r="G112" t="n">
         <v>277.22153234181</v>
       </c>
       <c r="H112" t="n">
-        <v>211.5260948773989</v>
+        <v>210.8520401185984</v>
       </c>
       <c r="I112" t="n">
         <v>39.9</v>
@@ -5064,13 +5064,13 @@
         </is>
       </c>
       <c r="F113" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G113" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H113" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I113" t="n">
         <v>22</v>
@@ -5105,13 +5105,13 @@
         </is>
       </c>
       <c r="F114" t="n">
-        <v>213.8218184785356</v>
+        <v>213.2007658469566</v>
       </c>
       <c r="G114" t="n">
         <v>0</v>
       </c>
       <c r="H114" t="n">
-        <v>213.8218184785356</v>
+        <v>213.2007658469566</v>
       </c>
       <c r="I114" t="n">
         <v>0</v>
@@ -5228,13 +5228,13 @@
         </is>
       </c>
       <c r="F117" t="n">
-        <v>494.6175539524428</v>
+        <v>496.846495637108</v>
       </c>
       <c r="G117" t="n">
         <v>277.22153234181</v>
       </c>
       <c r="H117" t="n">
-        <v>211.5202542701893</v>
+        <v>210.8466250273695</v>
       </c>
       <c r="I117" t="n">
         <v>39.9</v>
@@ -5269,13 +5269,13 @@
         </is>
       </c>
       <c r="F118" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G118" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H118" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I118" t="n">
         <v>21.3</v>
@@ -5310,13 +5310,13 @@
         </is>
       </c>
       <c r="F119" t="n">
-        <v>213.9854617004913</v>
+        <v>213.3627410968443</v>
       </c>
       <c r="G119" t="n">
         <v>0</v>
       </c>
       <c r="H119" t="n">
-        <v>213.9854617004913</v>
+        <v>213.3627410968443</v>
       </c>
       <c r="I119" t="n">
         <v>0</v>

</xml_diff>